<commit_message>
- [New] Support GetColumns method #174
</commit_message>
<xml_diff>
--- a/samples/xlsx/TestTemplateEasyFill.xlsx
+++ b/samples/xlsx/TestTemplateEasyFill.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\MiniExcel\samples\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A181A9-FD03-4C8E-83D0-BF48B594CB94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E86117-BB36-47D9-98BE-1A08B13E5028}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{1FA1D28D-370B-47FE-B520-FD158F1A8196}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{1FA1D28D-370B-47FE-B520-FD158F1A8196}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -441,7 +441,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,5 +489,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>